<commit_message>
feat: update data file and remove temporary backup file
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\dbw\Reown-appkit-EVM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d76eed7cb378b35/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F08CE96-1618-434A-8213-D089AF4BE4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C0220E0D-6976-47C7-B9E0-C92E5E0D9DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-3090" windowWidth="19380" windowHeight="10260" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="84">
   <si>
     <t>2 RHODIUM</t>
   </si>
@@ -110,6 +110,15 @@
     <t>Public Blog</t>
   </si>
   <si>
+    <t>Librairy</t>
+  </si>
+  <si>
+    <t>Dictionairy</t>
+  </si>
+  <si>
+    <t>Video Librairy</t>
+  </si>
+  <si>
     <t>Courses</t>
   </si>
   <si>
@@ -140,21 +149,12 @@
     <t>Minimum cashback in FLR</t>
   </si>
   <si>
-    <t>Cashback guarentee</t>
-  </si>
-  <si>
     <t>NFT Cashback</t>
   </si>
   <si>
     <t>Up to 100%</t>
   </si>
   <si>
-    <t>Up to 50%</t>
-  </si>
-  <si>
-    <t>Up to 40%</t>
-  </si>
-  <si>
     <t>Up to 30%</t>
   </si>
   <si>
@@ -194,15 +194,9 @@
     <t xml:space="preserve">Free Draws </t>
   </si>
   <si>
-    <t>Other sweepstake lots</t>
-  </si>
-  <si>
     <t>Bi Weekly FLR Sweepstakes</t>
   </si>
   <si>
-    <t>35% profit share pool</t>
-  </si>
-  <si>
     <t>Income streams</t>
   </si>
   <si>
@@ -269,13 +263,52 @@
     <t>E-Books</t>
   </si>
   <si>
-    <t>Video Library</t>
-  </si>
-  <si>
-    <t>Dictionary</t>
-  </si>
-  <si>
-    <t>Library</t>
+    <t>Other sweepstake Tickets</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cashback guarentee</t>
+    </r>
+  </si>
+  <si>
+    <t>Up to 25%</t>
+  </si>
+  <si>
+    <t>Up to 15%</t>
+  </si>
+  <si>
+    <t>Payout Frequency</t>
+  </si>
+  <si>
+    <t>Montly</t>
+  </si>
+  <si>
+    <t>Quartely</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>35% of Sweepstake pools</t>
   </si>
 </sst>
 </file>
@@ -285,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +330,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,6 +455,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,6 +480,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,17 +805,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="11" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
+    <col min="2" max="11" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -785,7 +847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -817,7 +879,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -829,7 +891,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -861,7 +923,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -893,7 +955,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -925,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -948,16 +1010,16 @@
         <v>11</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -989,7 +1051,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -1022,7 +1084,7 @@
       </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1086,7 +1148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1118,9 +1180,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>11</v>
@@ -1150,9 +1212,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>11</v>
@@ -1182,9 +1244,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>11</v>
@@ -1214,9 +1276,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>17</v>
@@ -1246,7 +1308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1278,9 +1340,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>11</v>
@@ -1310,39 +1372,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1354,9 +1416,9 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B21" s="12">
         <v>1</v>
@@ -1373,22 +1435,22 @@
       <c r="F21" s="12">
         <v>1</v>
       </c>
-      <c r="G21" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H21" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="I21" s="12">
+      <c r="G21" s="17">
         <v>0.3</v>
       </c>
-      <c r="J21" s="12">
+      <c r="H21" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="I21" s="17">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12">
         <v>0.75</v>
@@ -1405,22 +1467,22 @@
       <c r="F22" s="12">
         <v>0.75</v>
       </c>
-      <c r="G22" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="G22" s="17">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H22" s="17">
         <v>0.2</v>
       </c>
-      <c r="I22" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="J22" s="12">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="17">
+        <v>0.16</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>11</v>
@@ -1450,51 +1512,71 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
         <v>44</v>
       </c>
@@ -1526,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>45</v>
       </c>
@@ -1558,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1570,7 +1652,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>47</v>
       </c>
@@ -1602,7 +1684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
@@ -1634,7 +1716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1646,9 +1728,9 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
@@ -1678,7 +1760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1710,9 +1792,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="9">
         <v>30000</v>
@@ -1733,18 +1815,18 @@
         <v>938</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="9">
         <v>30000</v>
@@ -1765,18 +1847,18 @@
         <v>938</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="9">
         <v>24000</v>
@@ -1794,21 +1876,21 @@
         <v>1500</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="9">
         <v>24000</v>
@@ -1823,22 +1905,22 @@
         <v>3000</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1850,9 +1932,9 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>7</v>
@@ -1882,7 +1964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>49</v>
       </c>
@@ -1901,20 +1983,12 @@
       <c r="F40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>50</v>
       </c>
@@ -1946,7 +2020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>51</v>
       </c>
@@ -1978,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1990,9 +2064,9 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>52</v>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
@@ -2022,9 +2096,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B45" s="11">
         <v>6</v>
@@ -2054,9 +2128,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" s="11">
         <v>6</v>
@@ -2086,9 +2160,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B47" s="11">
         <v>6</v>
@@ -2118,9 +2192,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B48" s="11">
         <v>6</v>
@@ -2150,9 +2224,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B49" s="11">
         <v>6</v>
@@ -2182,9 +2256,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B50" s="11">
         <v>6</v>
@@ -2214,7 +2288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -2226,9 +2300,9 @@
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>54</v>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B52" s="12">
         <v>0.1</v>
@@ -2258,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2270,39 +2344,39 @@
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H54" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="I54" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -2314,9 +2388,9 @@
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>11</v>
@@ -2346,7 +2420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -2358,39 +2432,39 @@
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A58" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: enhance comparison table formatting and add JSX support for yes/no values
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dillo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A387C27-EF62-4FDC-B75F-F9750AAC989E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD2313C-8C16-42B1-A901-658ADBC6E7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
+    <workbookView xWindow="9510" yWindow="-3090" windowWidth="19380" windowHeight="10260" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>dillon devera</author>
+  </authors>
+  <commentList>
+    <comment ref="J44" authorId="0" shapeId="0" xr:uid="{F3F31D37-7521-41B9-99DB-F0F2190B6353}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dillon devera:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="87">
   <si>
     <t>2 RHODIUM</t>
   </si>
@@ -200,12 +234,6 @@
     <t>Income streams</t>
   </si>
   <si>
-    <t>5 to 10</t>
-  </si>
-  <si>
-    <t>2 to 7</t>
-  </si>
-  <si>
     <t>Giveaways</t>
   </si>
   <si>
@@ -242,19 +270,10 @@
     <t>Contibutor Access</t>
   </si>
   <si>
-    <t>3 to 8</t>
-  </si>
-  <si>
     <t>DBWF Token</t>
   </si>
   <si>
     <t>DBWL Token</t>
-  </si>
-  <si>
-    <t>7 to 12</t>
-  </si>
-  <si>
-    <t>PARTIAL</t>
   </si>
   <si>
     <t>E-Books</t>
@@ -311,9 +330,6 @@
     <t>10 SILVER</t>
   </si>
   <si>
-    <t>1 to 7</t>
-  </si>
-  <si>
     <t>6 Monthly</t>
   </si>
   <si>
@@ -323,7 +339,39 @@
     <t>Total price in USD</t>
   </si>
   <si>
-    <t xml:space="preserve"> YES</t>
+    <t>YES/PARTIAL</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -334,7 +382,7 @@
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-45C]#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,13 +413,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -425,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -485,6 +565,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,11 +929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -907,39 +1017,39 @@
         <v>13</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B4" s="23">
         <v>9600</v>
@@ -1064,16 +1174,16 @@
       <c r="G7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="14" t="s">
+      <c r="H7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="26" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1429,7 +1539,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -1582,7 +1692,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>11</v>
@@ -1638,27 +1748,27 @@
         <v>39</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="J24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>31</v>
@@ -1673,16 +1783,16 @@
         <v>31</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1827,7 @@
         <v>9</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1853,7 +1963,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
@@ -1923,7 +2033,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B34" s="7">
         <v>30000</v>
@@ -1944,21 +2054,21 @@
         <v>938</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" s="7">
         <v>30000</v>
@@ -1979,21 +2089,21 @@
         <v>938</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B36" s="7">
         <v>24000</v>
@@ -2011,24 +2121,24 @@
         <v>1500</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" s="7">
         <v>24000</v>
@@ -2043,22 +2153,22 @@
         <v>3000</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2106,7 +2216,7 @@
         <v>9</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2128,11 +2238,21 @@
       <c r="F40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="13"/>
+      <c r="G40" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="K40" s="33" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -2173,20 +2293,20 @@
       <c r="A42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="9">
-        <v>12</v>
-      </c>
-      <c r="C42" s="9">
-        <v>12</v>
-      </c>
-      <c r="D42" s="9">
-        <v>12</v>
-      </c>
-      <c r="E42" s="9">
-        <v>12</v>
-      </c>
-      <c r="F42" s="9">
-        <v>12</v>
+      <c r="B42" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C42" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D42" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E42" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F42" s="25">
+        <v>2025</v>
       </c>
       <c r="G42" s="9">
         <v>0</v>
@@ -2219,247 +2339,247 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K44" s="20" t="s">
-        <v>11</v>
+        <v>69</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J44" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="K44" s="28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="9">
-        <v>6</v>
-      </c>
-      <c r="C45" s="9">
-        <v>6</v>
-      </c>
-      <c r="D45" s="9">
-        <v>6</v>
-      </c>
-      <c r="E45" s="9">
-        <v>6</v>
-      </c>
-      <c r="F45" s="9">
-        <v>6</v>
-      </c>
-      <c r="G45" s="9">
-        <v>5</v>
-      </c>
-      <c r="H45" s="9">
-        <v>4</v>
-      </c>
-      <c r="I45" s="9">
-        <v>3</v>
-      </c>
-      <c r="J45" s="9">
-        <v>2</v>
-      </c>
-      <c r="K45" s="14">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="B45" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C45" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D45" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E45" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F45" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="9">
-        <v>6</v>
-      </c>
-      <c r="C46" s="9">
-        <v>6</v>
-      </c>
-      <c r="D46" s="9">
-        <v>6</v>
-      </c>
-      <c r="E46" s="9">
-        <v>6</v>
-      </c>
-      <c r="F46" s="9">
-        <v>6</v>
-      </c>
-      <c r="G46" s="9">
-        <v>5</v>
-      </c>
-      <c r="H46" s="9">
-        <v>4</v>
-      </c>
-      <c r="I46" s="9">
-        <v>3</v>
-      </c>
-      <c r="J46" s="9">
-        <v>2</v>
-      </c>
-      <c r="K46" s="14">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="B46" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C46" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D46" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E46" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F46" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H46" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K46" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="9">
-        <v>6</v>
-      </c>
-      <c r="C47" s="9">
-        <v>6</v>
-      </c>
-      <c r="D47" s="9">
-        <v>6</v>
-      </c>
-      <c r="E47" s="9">
-        <v>6</v>
-      </c>
-      <c r="F47" s="9">
-        <v>6</v>
-      </c>
-      <c r="G47" s="9">
-        <v>5</v>
-      </c>
-      <c r="H47" s="9">
-        <v>4</v>
-      </c>
-      <c r="I47" s="9">
-        <v>3</v>
-      </c>
-      <c r="J47" s="9">
-        <v>2</v>
-      </c>
-      <c r="K47" s="14">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="B47" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C47" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D47" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E47" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F47" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I47" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K47" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="9">
-        <v>6</v>
-      </c>
-      <c r="C48" s="9">
-        <v>6</v>
-      </c>
-      <c r="D48" s="9">
-        <v>6</v>
-      </c>
-      <c r="E48" s="9">
-        <v>6</v>
-      </c>
-      <c r="F48" s="9">
-        <v>6</v>
-      </c>
-      <c r="G48" s="9">
-        <v>5</v>
-      </c>
-      <c r="H48" s="9">
-        <v>4</v>
-      </c>
-      <c r="I48" s="9">
-        <v>3</v>
-      </c>
-      <c r="J48" s="9">
-        <v>2</v>
-      </c>
-      <c r="K48" s="14">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="B48" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C48" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D48" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E48" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F48" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K48" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="9">
-        <v>6</v>
-      </c>
-      <c r="C49" s="9">
-        <v>6</v>
-      </c>
-      <c r="D49" s="9">
-        <v>6</v>
-      </c>
-      <c r="E49" s="9">
-        <v>6</v>
-      </c>
-      <c r="F49" s="9">
-        <v>6</v>
-      </c>
-      <c r="G49" s="9">
-        <v>5</v>
-      </c>
-      <c r="H49" s="9">
-        <v>4</v>
-      </c>
-      <c r="I49" s="9">
-        <v>3</v>
-      </c>
-      <c r="J49" s="9">
-        <v>2</v>
-      </c>
-      <c r="K49" s="14">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B49" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C49" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D49" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E49" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F49" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="9">
-        <v>6</v>
-      </c>
-      <c r="C50" s="9">
-        <v>6</v>
-      </c>
-      <c r="D50" s="9">
-        <v>6</v>
-      </c>
-      <c r="E50" s="9">
-        <v>6</v>
-      </c>
-      <c r="F50" s="9">
-        <v>6</v>
-      </c>
-      <c r="G50" s="9">
-        <v>5</v>
-      </c>
-      <c r="H50" s="9">
-        <v>4</v>
-      </c>
-      <c r="I50" s="9">
-        <v>3</v>
-      </c>
-      <c r="J50" s="9">
-        <v>2</v>
-      </c>
-      <c r="K50" s="14">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B50" s="25">
+        <v>2025</v>
+      </c>
+      <c r="C50" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D50" s="25">
+        <v>2025</v>
+      </c>
+      <c r="E50" s="25">
+        <v>2025</v>
+      </c>
+      <c r="F50" s="25">
+        <v>2025</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I50" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K50" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2477,7 +2597,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B52" s="10">
         <v>0.1</v>
@@ -2527,35 +2647,35 @@
       <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I54" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J54" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>84</v>
+      <c r="B54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="H54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="J54" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K54" s="30" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2573,7 +2693,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>11</v>
@@ -2621,42 +2741,43 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>72</v>
+      <c r="C58" s="24" t="s">
+        <v>82</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update dashboard layout and improve tier display
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dillo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\dbw\Reown-appkit-EVM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD2313C-8C16-42B1-A901-658ADBC6E7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5EB0BD-5DAE-4AB9-AE20-7766A4A1B867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-3090" windowWidth="19380" windowHeight="10260" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="83">
   <si>
     <t>2 RHODIUM</t>
   </si>
@@ -168,15 +168,6 @@
     <t>Monthly</t>
   </si>
   <si>
-    <t>Per 2 months</t>
-  </si>
-  <si>
-    <t>Per 3 months</t>
-  </si>
-  <si>
-    <t>Per 6 Months</t>
-  </si>
-  <si>
     <t>Max cashback in FLR</t>
   </si>
   <si>
@@ -184,15 +175,6 @@
   </si>
   <si>
     <t>NFT Cashback</t>
-  </si>
-  <si>
-    <t>Up to 100%</t>
-  </si>
-  <si>
-    <t>Up to 30%</t>
-  </si>
-  <si>
-    <t>Up to 20%</t>
   </si>
   <si>
     <t>Knowledge tests</t>
@@ -306,12 +288,6 @@
     </r>
   </si>
   <si>
-    <t>Up to 25%</t>
-  </si>
-  <si>
-    <t>Up to 15%</t>
-  </si>
-  <si>
     <t>Payout Frequency</t>
   </si>
   <si>
@@ -322,9 +298,6 @@
   </si>
   <si>
     <t>35% of Sweepstake pools</t>
-  </si>
-  <si>
-    <t>Up to 10%</t>
   </si>
   <si>
     <t>10 SILVER</t>
@@ -372,6 +345,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 GOLD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6 Months</t>
+  </si>
+  <si>
+    <t>6 Months</t>
   </si>
 </sst>
 </file>
@@ -505,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,6 +583,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
@@ -974,12 +968,12 @@
         <v>9</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3">
         <v>25</v>
@@ -1017,39 +1011,39 @@
         <v>13</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B4" s="23">
         <v>9600</v>
@@ -1189,7 +1183,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8" s="7">
         <v>32000</v>
@@ -1224,7 +1218,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>11</v>
@@ -1504,7 +1498,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>11</v>
@@ -1539,7 +1533,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -1586,25 +1580,25 @@
         <v>31</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1622,7 +1616,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" s="10">
         <v>1</v>
@@ -1657,7 +1651,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="10">
         <v>0.75</v>
@@ -1692,7 +1686,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>11</v>
@@ -1727,48 +1721,48 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="B24" s="34">
+        <v>1</v>
+      </c>
+      <c r="C24" s="34">
+        <v>1</v>
+      </c>
+      <c r="D24" s="34">
+        <v>1</v>
+      </c>
+      <c r="E24" s="34">
+        <v>1</v>
+      </c>
+      <c r="F24" s="34">
+        <v>1</v>
+      </c>
+      <c r="G24" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="H24" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="J24" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="K24" s="35">
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>31</v>
@@ -1783,21 +1777,21 @@
         <v>31</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>7</v>
@@ -1827,12 +1821,12 @@
         <v>9</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B27" s="10">
         <v>0.1</v>
@@ -1880,7 +1874,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>11</v>
@@ -1915,7 +1909,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>11</v>
@@ -1963,7 +1957,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
@@ -1998,7 +1992,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B33" s="7">
         <v>32000</v>
@@ -2033,7 +2027,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B34" s="7">
         <v>30000</v>
@@ -2054,21 +2048,21 @@
         <v>938</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B35" s="7">
         <v>30000</v>
@@ -2089,21 +2083,21 @@
         <v>938</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7">
         <v>24000</v>
@@ -2121,24 +2115,24 @@
         <v>1500</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B37" s="7">
         <v>24000</v>
@@ -2153,22 +2147,22 @@
         <v>3000</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2186,7 +2180,7 @@
     </row>
     <row r="39" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>7</v>
@@ -2216,12 +2210,12 @@
         <v>9</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>11</v>
@@ -2239,24 +2233,24 @@
         <v>11</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>11</v>
@@ -2291,7 +2285,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B42" s="25">
         <v>2025</v>
@@ -2339,7 +2333,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>11</v>
@@ -2357,24 +2351,24 @@
         <v>11</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H44" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K44" s="28" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B45" s="25">
         <v>2025</v>
@@ -2392,24 +2386,24 @@
         <v>2025</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I45" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B46" s="25">
         <v>2025</v>
@@ -2427,24 +2421,24 @@
         <v>2025</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J46" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K46" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B47" s="25">
         <v>2025</v>
@@ -2462,24 +2456,24 @@
         <v>2025</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I47" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J47" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K47" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B48" s="25">
         <v>2025</v>
@@ -2497,24 +2491,24 @@
         <v>2025</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I48" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K48" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B49" s="25">
         <v>2025</v>
@@ -2532,24 +2526,24 @@
         <v>2025</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H49" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I49" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J49" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K49" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B50" s="25">
         <v>2025</v>
@@ -2567,19 +2561,19 @@
         <v>2025</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I50" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J50" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2597,7 +2591,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B52" s="10">
         <v>0.1</v>
@@ -2645,37 +2639,37 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J54" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K54" s="30" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2693,7 +2687,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>11</v>
@@ -2741,37 +2735,37 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chore: update data.xlsx with latest information
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\dbw\Reown-appkit-EVM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5EB0BD-5DAE-4AB9-AE20-7766A4A1B867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A1EFF5-8829-4A03-9BCD-8D86AEA1BD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="81">
   <si>
     <t>2 RHODIUM</t>
   </si>
@@ -241,12 +241,6 @@
   </si>
   <si>
     <t>Token Drops</t>
-  </si>
-  <si>
-    <t>TDB Token</t>
-  </si>
-  <si>
-    <t>DRKET Token</t>
   </si>
   <si>
     <t>Contibutor Access</t>
@@ -926,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
@@ -968,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1011,39 +1005,39 @@
         <v>13</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="23">
         <v>9600</v>
@@ -1533,7 +1527,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -1580,25 +1574,25 @@
         <v>31</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="I19" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1686,7 +1680,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>11</v>
@@ -1756,13 +1750,13 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>31</v>
@@ -1777,16 +1771,16 @@
         <v>31</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1821,7 +1815,7 @@
         <v>9</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2026,78 +2020,34 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="7">
-        <v>30000</v>
-      </c>
-      <c r="C34" s="7">
-        <v>15000</v>
-      </c>
-      <c r="D34" s="7">
-        <v>7500</v>
-      </c>
-      <c r="E34" s="7">
-        <v>3750</v>
-      </c>
-      <c r="F34" s="7">
-        <v>1875</v>
-      </c>
-      <c r="G34" s="7">
-        <v>938</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="18"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="7">
-        <v>30000</v>
-      </c>
-      <c r="C35" s="7">
-        <v>15000</v>
-      </c>
-      <c r="D35" s="7">
-        <v>7500</v>
-      </c>
-      <c r="E35" s="7">
-        <v>3750</v>
-      </c>
-      <c r="F35" s="7">
-        <v>1875</v>
-      </c>
-      <c r="G35" s="7">
-        <v>938</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="A35" s="4"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="18"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="7">
         <v>24000</v>
@@ -2132,7 +2082,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="7">
         <v>24000</v>
@@ -2210,7 +2160,7 @@
         <v>9</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2233,19 +2183,19 @@
         <v>11</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2333,7 +2283,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>11</v>
@@ -2386,7 +2336,7 @@
         <v>2025</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H45" s="25" t="s">
         <v>49</v>
@@ -2591,7 +2541,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52" s="10">
         <v>0.1</v>
@@ -2642,34 +2592,34 @@
         <v>47</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J54" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K54" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2735,13 +2685,13 @@
     </row>
     <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
chore: update data.xlsx with new contributor information
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\dbw\Reown-appkit-EVM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B923D858-4E7D-4E81-B6D2-C19AB0205B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD13A09-01CF-4820-959A-0D8A3D561763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75045D33-8362-430C-B375-83C72F4FE043}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="82">
   <si>
     <t>2 RHODIUM</t>
   </si>
@@ -490,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,9 +585,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -926,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA83995E-D196-4E19-8146-1590B424B7F4}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,39 +1179,17 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="7">
-        <v>32000</v>
-      </c>
-      <c r="C8" s="7">
-        <v>16000</v>
-      </c>
-      <c r="D8" s="7">
-        <v>8000</v>
-      </c>
-      <c r="E8" s="7">
-        <v>4000</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2000</v>
-      </c>
-      <c r="G8" s="7">
-        <v>800</v>
-      </c>
-      <c r="H8" s="7">
-        <v>400</v>
-      </c>
-      <c r="I8" s="7">
-        <v>200</v>
-      </c>
-      <c r="J8" s="7">
-        <v>100</v>
-      </c>
-      <c r="K8" s="18">
-        <v>50</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2037,7 +2012,7 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="36"/>
+      <c r="L34" s="7"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -2108,7 +2083,7 @@
       <c r="K36" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L36" s="36"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -2144,7 +2119,7 @@
       <c r="K37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L37" s="36"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -2180,7 +2155,7 @@
       <c r="K38" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L38" s="36"/>
+      <c r="L38" s="7"/>
     </row>
     <row r="39" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">

</xml_diff>